<commit_message>
xls2xml - bugfixes box
</commit_message>
<xml_diff>
--- a/xls2xml/tests_vivo/input_vivo.xlsx
+++ b/xls2xml/tests_vivo/input_vivo.xlsx
@@ -43,7 +43,7 @@
     <t xml:space="preserve">Genre 2</t>
   </si>
   <si>
-    <t xml:space="preserve">Série</t>
+    <t xml:space="preserve">Season</t>
   </si>
   <si>
     <t xml:space="preserve">Title</t>
@@ -945,11 +945,11 @@
   </sheetPr>
   <dimension ref="A1:AP35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W1" colorId="64" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z9" activeCellId="0" sqref="Z9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.38"/>

</xml_diff>